<commit_message>
Replace GET method body to RequestParams, add MainCategoryModelTransformer, SubCategoryModelTransformer null checks to domain object transfomrs
</commit_message>
<xml_diff>
--- a/budgetmanager-transaction-service/notes/constraints.xlsx
+++ b/budgetmanager-transaction-service/notes/constraints.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Istvan_Bartuszek\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\budget-manager\transaction-service\budget-manager\budgetmanager-transaction-service\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F2BB22F-2628-4B99-A29A-08D2D8CF4434}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{244DFDD3-03DA-4B64-BD38-5C80C8B66395}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="58">
   <si>
     <t>transaction</t>
   </si>
@@ -205,9 +205,6 @@
   </si>
   <si>
     <t>delete()</t>
-  </si>
-  <si>
-    <t>At web layer mainCategories and transactions tranformations: validation main/subCategoryFields must not be null!!!</t>
   </si>
 </sst>
 </file>
@@ -584,10 +581,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G57"/>
+  <dimension ref="A1:G54"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="A58" sqref="A58"/>
+      <selection activeCell="A56" sqref="A56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1636,29 +1633,12 @@
         <v>29</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A56" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="B56" s="5"/>
-      <c r="C56" s="5"/>
-      <c r="D56" s="5"/>
-      <c r="E56" s="5"/>
-      <c r="F56" s="5"/>
-      <c r="G56" s="5"/>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A57" s="5"/>
-      <c r="B57" s="5"/>
-      <c r="C57" s="5"/>
-      <c r="D57" s="5"/>
-      <c r="E57" s="5"/>
-      <c r="F57" s="5"/>
-      <c r="G57" s="5"/>
-    </row>
   </sheetData>
-  <mergeCells count="20">
-    <mergeCell ref="A56:G57"/>
+  <mergeCells count="19">
+    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="B21:B22"/>
     <mergeCell ref="B52:B54"/>
     <mergeCell ref="A27:A54"/>
     <mergeCell ref="A3:A12"/>
@@ -1674,10 +1654,6 @@
     <mergeCell ref="B40:B41"/>
     <mergeCell ref="B44:B45"/>
     <mergeCell ref="B3:B5"/>
-    <mergeCell ref="B6:B8"/>
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="B17:B19"/>
-    <mergeCell ref="B21:B22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>